<commit_message>
updated excel file with missing subgroup for ID 220553
</commit_message>
<xml_diff>
--- a/sidp.xlsx
+++ b/sidp.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4917" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4916" uniqueCount="418">
   <si>
     <t>ID</t>
   </si>
@@ -1743,7 +1743,7 @@
   <dimension ref="A1:BG121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV19" sqref="AV19"/>
+      <selection activeCell="G21" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -9336,7 +9336,7 @@
         <v>220553</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C45" s="2">
         <v>42599</v>
@@ -9348,8 +9348,8 @@
         <v>59</v>
       </c>
       <c r="F45" s="1"/>
-      <c r="G45" s="1" t="s">
-        <v>108</v>
+      <c r="G45" s="1">
+        <v>4</v>
       </c>
       <c r="H45" s="2">
         <v>21211</v>
@@ -42037,7 +42037,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTIF('02-14-17 ANNA SIDP DATA'!B:B,B3)</f>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>60</v>
@@ -42045,43 +42045,43 @@
       <c r="C3" s="22"/>
       <c r="D3" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B3,'02-14-17 ANNA SIDP DATA'!M:M)</f>
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E3" s="21">
         <f>D3/('02-14-17 ANNA SIDP DATA'!L2*$A3)</f>
-        <v>9.420289855072464E-2</v>
+        <v>9.2592592592592587E-2</v>
       </c>
       <c r="F3" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B3,'02-14-17 ANNA SIDP DATA'!O:O)</f>
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="21">
         <f>F3/('02-14-17 ANNA SIDP DATA'!N2*$A3)</f>
-        <v>0.20807453416149069</v>
+        <v>0.20634920634920634</v>
       </c>
       <c r="H3" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B3,'02-14-17 ANNA SIDP DATA'!Q:Q)</f>
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I3" s="21">
         <f>H3/('02-14-17 ANNA SIDP DATA'!P2*$A3)</f>
-        <v>0.51863354037267084</v>
+        <v>0.50793650793650791</v>
       </c>
       <c r="J3" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B3,'02-14-17 ANNA SIDP DATA'!S:S)</f>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K3" s="21">
         <f>J3/('02-14-17 ANNA SIDP DATA'!R2*$A3)</f>
-        <v>0.10869565217391304</v>
+        <v>9.8765432098765427E-2</v>
       </c>
       <c r="L3" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B3,'02-14-17 ANNA SIDP DATA'!U:U)</f>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M3" s="21">
         <f>L3/('02-14-17 ANNA SIDP DATA'!T2*$A3)</f>
-        <v>0.13043478260869565</v>
+        <v>0.1308641975308642</v>
       </c>
       <c r="N3" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B3,'02-14-17 ANNA SIDP DATA'!W:W)</f>
@@ -42089,13 +42089,13 @@
       </c>
       <c r="O3" s="21">
         <f>N3/('02-14-17 ANNA SIDP DATA'!V2*$A3)</f>
-        <v>5.7065217391304345E-2</v>
+        <v>5.8333333333333334E-2</v>
       </c>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>COUNTIF('02-14-17 ANNA SIDP DATA'!B:B,B4)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>73</v>
@@ -42103,43 +42103,43 @@
       <c r="C4" s="22"/>
       <c r="D4" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!B:B,B4,'02-14-17 ANNA SIDP DATA'!U:U)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="21">
         <f>D4/('02-14-17 ANNA SIDP DATA'!V3*A4)</f>
-        <v>0.16875000000000001</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F4" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B4,'02-14-17 ANNA SIDP DATA'!O:O)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" s="21">
         <f>F4/('02-14-17 ANNA SIDP DATA'!N3*$A4)</f>
-        <v>0.1</v>
+        <v>0.10884353741496598</v>
       </c>
       <c r="H4" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B4,'02-14-17 ANNA SIDP DATA'!Q:Q)</f>
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="I4" s="21">
         <f>H4/('02-14-17 ANNA SIDP DATA'!P3*$A4)</f>
-        <v>0.45714285714285713</v>
+        <v>0.48299319727891155</v>
       </c>
       <c r="J4" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B4,'02-14-17 ANNA SIDP DATA'!S:S)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K4" s="21">
         <f>J4/('02-14-17 ANNA SIDP DATA'!R3*$A4)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.10582010582010581</v>
       </c>
       <c r="L4" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B4,'02-14-17 ANNA SIDP DATA'!U:U)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M4" s="21">
         <f>L4/('02-14-17 ANNA SIDP DATA'!T3*$A4)</f>
-        <v>0.15</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="N4" s="1">
         <f>SUMIF('02-14-17 ANNA SIDP DATA'!$B:$B,$B4,'02-14-17 ANNA SIDP DATA'!W:W)</f>
@@ -42147,7 +42147,7 @@
       </c>
       <c r="O4" s="21">
         <f>N4/('02-14-17 ANNA SIDP DATA'!V3*$A4)</f>
-        <v>5.6250000000000001E-2</v>
+        <v>5.3571428571428568E-2</v>
       </c>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">

</xml_diff>